<commit_message>
loop gelukt tm t+40, variables predicted gelukt
</commit_message>
<xml_diff>
--- a/PCAstatic/predicted_factors.xlsx
+++ b/PCAstatic/predicted_factors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,635 @@
         <v>0.6950452740777643</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-1.176894100314984</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.9718073002489132</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.7559138083643788</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.6066113125324666</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6345026302622966</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-1.072087177907424</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.096439639326848</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.6819189876017965</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.5618803076291261</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5764261429982923</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.9763115786953294</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-1.207726675246225</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.6075979120231604</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.5136521170518644</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5208830756188469</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-0.8897370166614702</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-1.305707862459764</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.5334028527569331</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.4624960754079565</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4679316172300229</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-0.8124734249392896</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-1.390504487161722</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.4597666470079855</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.4089688293555864</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.4176207378931381</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-0.7445722597629131</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.462315209742772</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.3871003819692676</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.3536115296813342</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.3699897315165518</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-0.6860281941169722</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-1.521411290990606</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.3157914958122781</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.2969471859040457</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3250678410306556</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-0.6367811637153002</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-1.568131540045202</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.2462021510578265</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.2394782503708764</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.2828739969856571</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>-0.5967187314197897</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-1.602877031686553</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.1786678655766301</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.1816844431480597</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2434166674154368</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>-0.5656787361682005</v>
+      </c>
+      <c r="B14" t="n">
+        <v>-1.626105640639881</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.1134963967288182</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.1240208221835252</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.2066938134236317</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>-0.5434521923392754</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-1.63832643957774</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.05096687367873359</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.06691610087488417</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.1726929443168985</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>-0.5297864055457613</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.640094006153804</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.008670828424104405</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.01077121331136172</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1413912657790639</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>-0.5243882711277141</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-1.632002682809781</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.06519648002942464</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.04404187428252296</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1127559143261726</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>-0.526927722109951</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-1.614680831283285</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.1184196633825611</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.09718110901556154</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.08674427108536481</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>-0.5370412940758494</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-1.588785121734031</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.1681797232767969</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1483350583642865</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.06330434779713882</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>-0.5543357752809851</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-1.554994894221553</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.2143455132833446</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1972233848586382</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.04237523784933599</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>-0.5783919113700275</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.514006627932998</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.2568149492372711</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2435970958241407</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.02388762511029154</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>-0.6087681352536994</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-1.466528551097458</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.2955143824933926</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.287238576790127</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.00776434333611957</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>-0.6450042940344232</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-1.41327542195655</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.330397806081717</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.3279614182597185</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.006079021019240961</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>-0.6866253463239721</v>
+      </c>
+      <c r="B24" t="n">
+        <v>-1.35496350851223</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.3614459073889499</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.3656100465036906</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.01773348966525264</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>-0.7331450048582806</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.292305792063734</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.3886649813732458</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.4000591698862715</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-0.02729602394289884</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>-0.784069300968209</v>
+      </c>
+      <c r="B26" t="n">
+        <v>-1.22600741679766</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.4120857185867082</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.4312130529564634</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.03486883365863979</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>-0.8389000491948315</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.156761404928951</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.4317618824378135</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.4590046311445458</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.04055866983115752</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>-0.8971381921285628</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-1.085244654125595</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.4477688901780442</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.4833944793917233</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.04447610765352367</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>-0.9582870073881783</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-1.012114231204905</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.4602023120483835</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.5043696484138029</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-0.04673482569994558</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>-1.021855160524071</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-0.9380039733821633</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.4691763028769866</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5219423825604057</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-0.04745088710671948</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>-1.087359589515613</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-0.8635214056994422</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.474821980185036</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.5361487333832291</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-0.04674202813469799</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>-1.154328208422041</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.7892449806793549</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.4772857625392292</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.5470470830745054</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-0.04472695917862338</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>-1.222302419626735</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.715721643749197</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.4767276814929286</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.5547165918848116</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.04152468293028572</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>-1.290839425973952</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.6434647255786926</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.4733196799900566</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5592555834829811</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.03725383403081328</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>-1.359514335923492</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-0.5729521601806157</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.4672439095729635</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.5607798819856011</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-0.03203204416554371</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>-1.427922056631754</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-0.5046250254487218</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.4586910381445302</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.5594211140654181</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.02597533616590496</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>-1.495678971597166</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-0.4388864007604267</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.4478585793924562</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.5553249891530734</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-0.01919755028947071</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>-1.562424401174931</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-0.3761005343604014</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.4349492542968535</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.5486495702814008</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.01180980545465659</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>-1.627821845862423</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-0.3165923114722077</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.4201693944177923</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.5395635475926213</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.003919997813106478</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>-1.691560013774554</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-0.2606470124631985</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.4037273959039603</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.5282445259428387</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.004367661346796284</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>-1.753353635162215</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-0.208510348917629</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.3858322323838531</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.5148773374021197</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.01295306675521412</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>